<commit_message>
fix inc directory error
</commit_message>
<xml_diff>
--- a/__doc/carl.xlsx
+++ b/__doc/carl.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8CE83A-E365-448C-ACB7-6F0FD587F4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="34110" yWindow="3255" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (3)" sheetId="5" r:id="rId1"/>
@@ -13,12 +14,28 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$B$1:$B$163</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>剑指offer29</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,11 +251,19 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -280,7 +305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,9 +337,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,6 +389,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,126 +582,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+    <sheetView topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1">
         <v>704</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>844</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>977</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B11">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>904</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B13">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B14">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B15">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18">
         <v>707</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B20">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -648,112 +709,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B23">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B24">
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B25">
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B26">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B27">
         <v>438</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B28">
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B29">
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B30">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>454</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B35">
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B36">
         <v>541</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B38">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B40">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B41">
         <v>459</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B44">
         <v>160</v>
       </c>
@@ -761,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B45">
         <v>232</v>
       </c>
@@ -769,7 +830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B46">
         <v>225</v>
       </c>
@@ -777,32 +838,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B47">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B48">
         <v>1047</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B49">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B50">
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B51">
         <v>347</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -810,82 +871,82 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B53">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B54">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B55">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B56">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B57">
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B58">
         <v>637</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B59">
         <v>429</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B60">
         <v>515</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B61">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B62">
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B63">
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B64">
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B65">
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B66">
         <v>589</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B67">
         <v>590</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -893,17 +954,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B69">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B70">
         <v>572</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -911,12 +972,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B72">
         <v>559</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -924,7 +985,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -932,7 +993,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -940,7 +1001,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -948,92 +1009,92 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B77">
         <v>404</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B78">
         <v>513</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B79">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B80">
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B81">
         <v>654</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B82">
         <v>617</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B83">
         <v>700</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B84">
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B85">
         <v>530</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B86">
         <v>501</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B87">
         <v>538</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B88">
         <v>236</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B89">
         <v>235</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B90">
         <v>701</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B91">
         <v>450</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B92">
         <v>669</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B93">
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -1041,77 +1102,77 @@
         <v>77</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B95">
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B96">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B97">
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B98">
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B99">
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B100">
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B101">
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B102">
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B103">
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B104">
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B105">
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B106">
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B107">
         <v>491</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B108">
         <v>332</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -1119,92 +1180,92 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B110">
         <v>1005</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B111">
         <v>860</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B112">
         <v>376</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B113">
         <v>738</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B114">
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B115">
         <v>714</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B116">
         <v>135</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B117">
         <v>406</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B118">
         <v>55</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B119">
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B120">
         <v>452</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B121">
         <v>435</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B122">
         <v>763</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B123">
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B124">
         <v>53</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B125">
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B126">
         <v>968</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -1212,172 +1273,172 @@
         <v>509</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B128">
         <v>70</v>
       </c>
     </row>
-    <row r="129" spans="2:2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B129">
         <v>746</v>
       </c>
     </row>
-    <row r="130" spans="2:2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B130">
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="2:2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B131">
         <v>63</v>
       </c>
     </row>
-    <row r="132" spans="2:2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B132">
         <v>343</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B133">
         <v>96</v>
       </c>
     </row>
-    <row r="134" spans="2:2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B134">
         <v>416</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B135">
         <v>1049</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B136">
         <v>494</v>
       </c>
     </row>
-    <row r="137" spans="2:2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B137">
         <v>474</v>
       </c>
     </row>
-    <row r="138" spans="2:2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B138">
         <v>518</v>
       </c>
     </row>
-    <row r="139" spans="2:2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B139">
         <v>377</v>
       </c>
     </row>
-    <row r="140" spans="2:2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B140">
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="2:2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B141">
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="2:2">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B142">
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="2:2">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B143">
         <v>198</v>
       </c>
     </row>
-    <row r="144" spans="2:2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B144">
         <v>213</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B145">
         <v>337</v>
       </c>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B146">
         <v>121</v>
       </c>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B147">
         <v>123</v>
       </c>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B148">
         <v>188</v>
       </c>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B149">
         <v>309</v>
       </c>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B150">
         <v>300</v>
       </c>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B151">
         <v>1143</v>
       </c>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B152">
         <v>1035</v>
       </c>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B153">
         <v>674</v>
       </c>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B154">
         <v>718</v>
       </c>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B155">
         <v>392</v>
       </c>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B156">
         <v>115</v>
       </c>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B157">
         <v>583</v>
       </c>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B158">
         <v>72</v>
       </c>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B159">
         <v>647</v>
       </c>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B160">
         <v>516</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -1385,12 +1446,12 @@
         <v>416</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B162">
         <v>297</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
         <v>21</v>
       </c>
@@ -1398,7 +1459,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
         <v>22</v>
       </c>
@@ -1406,382 +1467,382 @@
         <v>300</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B165">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B166">
         <v>141</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B167">
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B168">
         <v>189</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B169">
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B170">
         <v>88</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B171">
         <v>66</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B172">
         <v>155</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B173">
         <v>84</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B174">
         <v>641</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B175">
         <v>42</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B176">
         <v>144</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B177">
         <v>22</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B178">
         <v>105</v>
       </c>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B179">
         <v>50</v>
       </c>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B180">
         <v>169</v>
       </c>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B181">
         <v>433</v>
       </c>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B182">
         <v>127</v>
       </c>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B183">
         <v>126</v>
       </c>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B184">
         <v>200</v>
       </c>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B185">
         <v>529</v>
       </c>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B186">
         <v>455</v>
       </c>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B187">
         <v>874</v>
       </c>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B188">
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B189">
         <v>74</v>
       </c>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B190">
         <v>153</v>
       </c>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B192">
         <v>120</v>
       </c>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B193">
         <v>152</v>
       </c>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B194">
         <v>980</v>
       </c>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B195">
         <v>32</v>
       </c>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B196">
         <v>64</v>
       </c>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B197">
         <v>91</v>
       </c>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B198">
         <v>221</v>
       </c>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B199">
         <v>363</v>
       </c>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B200">
         <v>403</v>
       </c>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B201">
         <v>410</v>
       </c>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B202">
         <v>552</v>
       </c>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B203">
         <v>621</v>
       </c>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B204">
         <v>312</v>
       </c>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B205">
         <v>208</v>
       </c>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B206">
         <v>212</v>
       </c>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B207">
         <v>547</v>
       </c>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B208">
         <v>130</v>
       </c>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B209">
         <v>36</v>
       </c>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B210">
         <v>1263</v>
       </c>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B211">
         <v>1091</v>
       </c>
     </row>
-    <row r="212" spans="2:2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B212">
         <v>773</v>
       </c>
     </row>
-    <row r="213" spans="2:2">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B213">
         <v>109</v>
       </c>
     </row>
-    <row r="214" spans="2:2">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B214">
         <v>295</v>
       </c>
     </row>
-    <row r="215" spans="2:2">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B215">
         <v>327</v>
       </c>
     </row>
-    <row r="216" spans="2:2">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B216">
         <v>405</v>
       </c>
     </row>
-    <row r="217" spans="2:2">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B217">
         <v>191</v>
       </c>
     </row>
-    <row r="218" spans="2:2">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B218">
         <v>231</v>
       </c>
     </row>
-    <row r="219" spans="2:2">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B219">
         <v>190</v>
       </c>
     </row>
-    <row r="220" spans="2:2">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B220">
         <v>52</v>
       </c>
     </row>
-    <row r="221" spans="2:2">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B221">
         <v>338</v>
       </c>
     </row>
-    <row r="222" spans="2:2">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B222">
         <v>146</v>
       </c>
     </row>
-    <row r="223" spans="2:2">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B223">
         <v>1122</v>
       </c>
     </row>
-    <row r="224" spans="2:2">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B224">
         <v>1244</v>
       </c>
     </row>
-    <row r="225" spans="2:2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B225">
         <v>493</v>
       </c>
     </row>
-    <row r="226" spans="2:2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B226">
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="2:2">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B227">
         <v>818</v>
       </c>
     </row>
-    <row r="228" spans="2:2">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B228">
         <v>709</v>
       </c>
     </row>
-    <row r="229" spans="2:2">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B229">
         <v>58</v>
       </c>
     </row>
-    <row r="230" spans="2:2">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B230">
         <v>771</v>
       </c>
     </row>
-    <row r="231" spans="2:2">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B231">
         <v>387</v>
       </c>
     </row>
-    <row r="232" spans="2:2">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B232">
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="2:2">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B233">
         <v>14</v>
       </c>
     </row>
-    <row r="234" spans="2:2">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B234">
         <v>557</v>
       </c>
     </row>
-    <row r="235" spans="2:2">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B235">
         <v>917</v>
       </c>
     </row>
-    <row r="236" spans="2:2">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B236">
         <v>125</v>
       </c>
     </row>
-    <row r="237" spans="2:2">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B237">
         <v>680</v>
       </c>
     </row>
-    <row r="238" spans="2:2">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B238">
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="2:2">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B239">
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="2:2">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B240">
         <v>44</v>
       </c>
     </row>
-    <row r="241" spans="2:2">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B241">
         <v>205</v>
       </c>
@@ -1789,9 +1850,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B165:B241">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1799,126 +1860,126 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1">
         <v>704</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>844</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>977</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B11">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>904</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B13">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B14">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B15">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18">
         <v>707</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B20">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -1926,142 +1987,142 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B23">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B24">
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B25">
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B26">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B27">
         <v>438</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B28">
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B29">
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B30">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>454</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B33">
         <v>383</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B34">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B35">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B36">
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B37">
         <v>541</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B39">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B41">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B42">
         <v>459</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B43">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B44">
         <v>344</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B46">
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B47">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B48">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B50">
         <v>160</v>
       </c>
@@ -2069,22 +2130,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B51">
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B52">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B53">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B54">
         <v>232</v>
       </c>
@@ -2092,7 +2153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B55">
         <v>225</v>
       </c>
@@ -2100,32 +2161,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B56">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B57">
         <v>1047</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B58">
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B59">
         <v>239</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B60">
         <v>347</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -2133,82 +2194,82 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B62">
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B63">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B64">
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B65">
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B66">
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B67">
         <v>637</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B68">
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B69">
         <v>515</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B70">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B71">
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B72">
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B73">
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B74">
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B75">
         <v>589</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B76">
         <v>590</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -2216,17 +2277,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B78">
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B79">
         <v>572</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -2234,12 +2295,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B81">
         <v>559</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -2247,7 +2308,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -2255,7 +2316,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -2263,7 +2324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2271,92 +2332,92 @@
         <v>257</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B86">
         <v>404</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B87">
         <v>513</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B88">
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B89">
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B90">
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B91">
         <v>617</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B92">
         <v>700</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B93">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B94">
         <v>530</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B95">
         <v>501</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B96">
         <v>538</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B97">
         <v>236</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B98">
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B99">
         <v>701</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B100">
         <v>450</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B101">
         <v>669</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B102">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -2364,77 +2425,77 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B104">
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B105">
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B106">
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B107">
         <v>216</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B108">
         <v>131</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B109">
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B110">
         <v>78</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B111">
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B112">
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B113">
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B114">
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B115">
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B116">
         <v>491</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B117">
         <v>332</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -2442,92 +2503,92 @@
         <v>455</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B119">
         <v>1005</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B120">
         <v>860</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B121">
         <v>376</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B122">
         <v>738</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B123">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B124">
         <v>714</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B125">
         <v>135</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B126">
         <v>406</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B127">
         <v>55</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B128">
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B129">
         <v>452</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B130">
         <v>435</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B131">
         <v>763</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B132">
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B133">
         <v>53</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B134">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B135">
         <v>968</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -2535,192 +2596,192 @@
         <v>509</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B137">
         <v>70</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B138">
         <v>746</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B139">
         <v>62</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B140">
         <v>63</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B141">
         <v>343</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B142">
         <v>96</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B143">
         <v>416</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B144">
         <v>1049</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B145">
         <v>494</v>
       </c>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B146">
         <v>474</v>
       </c>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B147">
         <v>518</v>
       </c>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B148">
         <v>377</v>
       </c>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B149">
         <v>70</v>
       </c>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B150">
         <v>322</v>
       </c>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B151">
         <v>279</v>
       </c>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B152">
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B153">
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B154">
         <v>213</v>
       </c>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B155">
         <v>337</v>
       </c>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B156">
         <v>121</v>
       </c>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B157">
         <v>122</v>
       </c>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B158">
         <v>123</v>
       </c>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B159">
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B160">
         <v>309</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B161">
         <v>714</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B162">
         <v>300</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B163">
         <v>1143</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B164">
         <v>1035</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B165">
         <v>674</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B166">
         <v>718</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B167">
         <v>53</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B168">
         <v>392</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B169">
         <v>115</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B170">
         <v>583</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B171">
         <v>72</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B172">
         <v>647</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B173">
         <v>516</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -2728,52 +2789,52 @@
         <v>416</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B175">
         <v>1049</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B176">
         <v>494</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B177">
         <v>474</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B178">
         <v>518</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B179">
         <v>377</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B180">
         <v>70</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B181">
         <v>322</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B182">
         <v>297</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B183">
         <v>139</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
         <v>21</v>
       </c>
@@ -2781,32 +2842,32 @@
         <v>121</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B185">
         <v>122</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B186">
         <v>123</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B187">
         <v>188</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B188">
         <v>309</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B189">
         <v>714</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
         <v>22</v>
       </c>
@@ -2814,57 +2875,57 @@
         <v>300</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B191">
         <v>1143</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B192">
         <v>1035</v>
       </c>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B193">
         <v>674</v>
       </c>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B194">
         <v>718</v>
       </c>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B195">
         <v>53</v>
       </c>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B196">
         <v>392</v>
       </c>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B197">
         <v>115</v>
       </c>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B198">
         <v>583</v>
       </c>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B199">
         <v>72</v>
       </c>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B200">
         <v>647</v>
       </c>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B201">
         <v>516</v>
       </c>
@@ -2877,126 +2938,127 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C164"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="B164" sqref="B164"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1">
         <v>704</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>844</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>977</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B11">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>904</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B13">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B14">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B15">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18">
         <v>707</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B20">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -3004,778 +3066,1123 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B23">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B24">
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B25">
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B26">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B27">
         <v>438</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B28">
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B29">
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B30">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>454</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B35">
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B36">
         <v>541</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B38">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B40">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B41">
         <v>459</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
-      <c r="B43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B43">
+        <v>160</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B44">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B45">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B47">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B48">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B49">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B50">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B52">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B53">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B54">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B55">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B56">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B57">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B58">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B59">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B60">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B61">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B62">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B63">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B64">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B65">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B66">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B68">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B69">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B71">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B76">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B77">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B78">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B79">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B80">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B81">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B82">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B83">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B84">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B85">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B86">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B87">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B88">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B89">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B90">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B91">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B92">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B94">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B95">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B96">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B97">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B98">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B99">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B100">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B101">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B102">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B103">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B104">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B105">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B106">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B107">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B109">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B110">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B111">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B112">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B113">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B114">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B115">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B116">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B117">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B118">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B119">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B120">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B121">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B122">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B123">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B124">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B125">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B127">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B128">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B129">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B130">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B131">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B132">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B133">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B134">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B135">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B136">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B137">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B138">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B139">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B140">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B141">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B142">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B143">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B144">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B145">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B146">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B147">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B148">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B149">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B150">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B151">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B152">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B153">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B154">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B155">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B156">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B157">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B158">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B159">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A160" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B161">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A162" t="s">
+        <v>21</v>
+      </c>
+      <c r="B162">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A163" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B164">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B165">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B166">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B167">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B168">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B169">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B170">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B171">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B172">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B173">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B174">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B175">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B176">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B177">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B178">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B179">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B180">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B181">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B182">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B183">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B184">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B185">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B186">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B187">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B188">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B189">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B190">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B191">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B192">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B193">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B194">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B195">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B196">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B197">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B198">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B199">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B200">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B201">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B202">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B203">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B204">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B205">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B206">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B207">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B208">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B209">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B210">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B211">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B212">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B213">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B214">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B215">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B216">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B217">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B218">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B219">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B220">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B221">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B222">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B223">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
-      <c r="B46">
-        <v>225</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="B49">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="B50">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="B51">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B224">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B225">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B226">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B227">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B228">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B229">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B230">
         <v>10</v>
       </c>
-      <c r="B52">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="B53">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="B54">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="B55">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="B56">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="B57">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="B58">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="B59">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="B60">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="B61">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="B62">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="B63">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="B64">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="B65">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="B66">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="B67">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>11</v>
-      </c>
-      <c r="B68">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="B69">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="B70">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="B72">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
-        <v>15</v>
-      </c>
-      <c r="B74">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>16</v>
-      </c>
-      <c r="B76">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="B77">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="B78">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="B79">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="B80">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="B81">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="B82">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="B83">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="B84">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="B85">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="B86">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="B87">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="B88">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="B89">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="B90">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="B91">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="B92">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="B93">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>17</v>
-      </c>
-      <c r="B94">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="B95">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="B96">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="B97">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="B98">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="B99">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="B100">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="B101">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="B102">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="B103">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="B104">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="B105">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="B106">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="B107">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="B108">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
-        <v>18</v>
-      </c>
-      <c r="B109">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="B110">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="B111">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="B112">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="B113">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="B114">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="B115">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="B116">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="B117">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="B118">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="B119">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="B120">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="B121">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="B122">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="B123">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="B124">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="B125">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="B126">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" t="s">
-        <v>19</v>
-      </c>
-      <c r="B127">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="B128">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2">
-      <c r="B129">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2">
-      <c r="B130">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2">
-      <c r="B131">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2">
-      <c r="B132">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2">
-      <c r="B133">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2">
-      <c r="B134">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2">
-      <c r="B135">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2">
-      <c r="B136">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2">
-      <c r="B137">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2">
-      <c r="B138">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2">
-      <c r="B139">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2">
-      <c r="B140">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2">
-      <c r="B141">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2">
-      <c r="B142">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2">
-      <c r="B143">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2">
-      <c r="B144">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2">
-      <c r="B145">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2">
-      <c r="B146">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2">
-      <c r="B147">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2">
-      <c r="B148">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2">
-      <c r="B149">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="150" spans="2:2">
-      <c r="B150">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2">
-      <c r="B151">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2">
-      <c r="B152">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2">
-      <c r="B153">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2">
-      <c r="B154">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2">
-      <c r="B155">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2">
-      <c r="B156">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2">
-      <c r="B157">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2">
-      <c r="B158">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2">
-      <c r="B159">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2">
-      <c r="B160">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" t="s">
-        <v>20</v>
-      </c>
-      <c r="B161">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="B162">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" t="s">
-        <v>21</v>
-      </c>
-      <c r="B163">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" t="s">
-        <v>22</v>
-      </c>
-      <c r="B164">
-        <v>300</v>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B231">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B232">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B159:B232">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3784,12 +4191,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>